<commit_message>
fix: docs and n/a
</commit_message>
<xml_diff>
--- a/storage/temp/worksheet.xlsx
+++ b/storage/temp/worksheet.xlsx
@@ -11,15 +11,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>cos@gmail.com</t>
-  </si>
-  <si>
-    <t>gap</t>
-  </si>
-  <si>
-    <t>text</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>pierdoli</t>
+  </si>
+  <si>
+    <t>smiedzi</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>debil@gmail.com</t>
+  </si>
+  <si>
+    <t>no debil no</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>idiota@gmail.com</t>
+  </si>
+  <si>
+    <t>no idiota no</t>
   </si>
 </sst>
 </file>
@@ -396,24 +420,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>